<commit_message>
Primera graf act 2
</commit_message>
<xml_diff>
--- a/Efecto Hall/Efecto_Hall.xlsx
+++ b/Efecto Hall/Efecto_Hall.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24703"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1016E481-FDE6-4FF8-8F55-53207A8A576A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaalvarezlopez/Documents/Universidad/Noveno Semestre/Laboratorio Intermedio/Laboratorios/Efecto Hall/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0579A47D-E87B-C442-981A-8961494CAD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p V-I" sheetId="2" r:id="rId1"/>
@@ -32,24 +37,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
   <si>
     <t>Corriente (mA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltaje Hall a 2 A (mV) </t>
-  </si>
-  <si>
-    <t>Voltaje Hall a 2.25 A(mV)</t>
   </si>
   <si>
     <t>Voltaje Hall a 2,5 A (mV)</t>
   </si>
   <si>
     <t>Voltaje Hall a 1,75 A (mV)</t>
-  </si>
-  <si>
-    <t>Voltaje Hall a 1,5 A(mV)</t>
   </si>
   <si>
     <t>Voltaje Hall a 1,5 A (mV)</t>
@@ -102,12 +98,15 @@
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>Voltaje Hall a 2 A (mV)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,7 +162,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -461,656 +460,657 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAC1A5E-0125-4EDD-8B83-074940BBBEA3}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
       <c r="B2">
+        <v>54.3</v>
+      </c>
+      <c r="C2">
+        <v>59.4</v>
+      </c>
+      <c r="D2">
         <v>70.400000000000006</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>69.2</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>73.7</v>
       </c>
-      <c r="E2">
-        <v>59.4</v>
-      </c>
-      <c r="F2">
-        <v>54.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>28</v>
       </c>
       <c r="B3">
+        <v>49.8</v>
+      </c>
+      <c r="C3">
+        <v>53.4</v>
+      </c>
+      <c r="D3">
         <v>62</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>65.3</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>66</v>
       </c>
-      <c r="E3">
-        <v>53.4</v>
-      </c>
-      <c r="F3">
-        <v>49.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>26</v>
       </c>
       <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>51.8</v>
+      </c>
+      <c r="D4">
         <v>58.1</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>56.8</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>60.8</v>
       </c>
-      <c r="E4">
-        <v>51.8</v>
-      </c>
-      <c r="F4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
       <c r="B5">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="C5">
+        <v>43.3</v>
+      </c>
+      <c r="D5">
         <v>50.8</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>51</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>55.3</v>
       </c>
-      <c r="E5">
-        <v>43.3</v>
-      </c>
-      <c r="F5">
-        <v>40.799999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>22</v>
       </c>
       <c r="B6">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="C6">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D6">
         <v>44.7</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>48.8</v>
       </c>
-      <c r="E6">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="F6">
-        <v>33.700000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7">
+        <v>28.8</v>
+      </c>
+      <c r="C7">
+        <v>34.1</v>
+      </c>
+      <c r="D7">
         <v>38.700000000000003</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>40.299999999999997</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>42.9</v>
       </c>
-      <c r="E7">
-        <v>34.1</v>
-      </c>
-      <c r="F7">
-        <v>28.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>18</v>
       </c>
       <c r="B8">
+        <v>23.7</v>
+      </c>
+      <c r="C8">
+        <v>26.5</v>
+      </c>
+      <c r="D8">
         <v>33.6</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>33.200000000000003</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>36.1</v>
       </c>
-      <c r="E8">
-        <v>26.5</v>
-      </c>
-      <c r="F8">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
       <c r="B9">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="C9">
+        <v>22.6</v>
+      </c>
+      <c r="D9">
         <v>28.1</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>26.2</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>31.7</v>
       </c>
-      <c r="E9">
-        <v>22.6</v>
-      </c>
-      <c r="F9">
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>14</v>
       </c>
       <c r="B10">
+        <v>14.2</v>
+      </c>
+      <c r="C10">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D10">
         <v>22.2</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>19.399999999999999</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>25</v>
       </c>
-      <c r="E10">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="F10">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12</v>
       </c>
       <c r="B11">
+        <v>9.4</v>
+      </c>
+      <c r="C11">
+        <v>11.4</v>
+      </c>
+      <c r="D11">
         <v>16</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>14.8</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>18.5</v>
       </c>
-      <c r="E11">
-        <v>11.4</v>
-      </c>
-      <c r="F11">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C12">
+        <v>7.5</v>
+      </c>
+      <c r="D12">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>11.1</v>
       </c>
-      <c r="E12">
-        <v>7.5</v>
-      </c>
-      <c r="F12">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8</v>
       </c>
       <c r="B13">
+        <v>-0.8</v>
+      </c>
+      <c r="C13">
+        <v>-0.7</v>
+      </c>
+      <c r="D13">
         <v>2.8</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>4.8</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>4.7</v>
       </c>
-      <c r="E13">
-        <v>-0.7</v>
-      </c>
-      <c r="F13">
-        <v>-0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
+        <v>-5.2</v>
+      </c>
+      <c r="C14">
+        <v>-4.8</v>
+      </c>
+      <c r="D14">
         <v>-3.8</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>-2.9</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>-0.4</v>
       </c>
-      <c r="E14">
-        <v>-4.8</v>
-      </c>
-      <c r="F14">
-        <v>-5.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15">
+        <v>-11.2</v>
+      </c>
+      <c r="C15">
+        <v>-11.3</v>
+      </c>
+      <c r="D15">
         <v>-9.1</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>-10</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>-6.9</v>
       </c>
-      <c r="E15">
-        <v>-11.3</v>
-      </c>
-      <c r="F15">
-        <v>-11.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16">
+        <v>-17.2</v>
+      </c>
+      <c r="C16">
+        <v>-18</v>
+      </c>
+      <c r="D16">
         <v>-15.2</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>-16.8</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>-15.1</v>
       </c>
-      <c r="E16">
-        <v>-18</v>
-      </c>
-      <c r="F16">
-        <v>-17.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
       <c r="B17">
+        <v>-19.7</v>
+      </c>
+      <c r="C17">
+        <v>-24.5</v>
+      </c>
+      <c r="D17">
         <v>-20.2</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>-25.8</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>-20.9</v>
       </c>
-      <c r="E17">
-        <v>-24.5</v>
-      </c>
-      <c r="F17">
-        <v>-19.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-2</v>
       </c>
       <c r="B18">
+        <v>-28</v>
+      </c>
+      <c r="C18">
+        <v>-32.200000000000003</v>
+      </c>
+      <c r="D18">
         <v>-29.5</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>-33.700000000000003</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>-29.7</v>
       </c>
-      <c r="E18">
-        <v>-32.200000000000003</v>
-      </c>
-      <c r="F18">
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-4</v>
       </c>
       <c r="B19">
+        <v>-34.299999999999997</v>
+      </c>
+      <c r="C19">
+        <v>-36.700000000000003</v>
+      </c>
+      <c r="D19">
         <v>-36.6</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>-39.700000000000003</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>-38.799999999999997</v>
       </c>
-      <c r="E19">
-        <v>-36.700000000000003</v>
-      </c>
-      <c r="F19">
-        <v>-34.299999999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-6</v>
       </c>
       <c r="B20">
+        <v>-40.4</v>
+      </c>
+      <c r="C20">
+        <v>-42.8</v>
+      </c>
+      <c r="D20">
         <v>-41.4</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>-46.3</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>-43.2</v>
       </c>
-      <c r="E20">
-        <v>-42.8</v>
-      </c>
-      <c r="F20">
-        <v>-40.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-8</v>
       </c>
       <c r="B21">
+        <v>-46.4</v>
+      </c>
+      <c r="C21">
+        <v>-48.5</v>
+      </c>
+      <c r="D21">
         <v>-46</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <v>-50.7</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>-52.9</v>
       </c>
-      <c r="E21">
-        <v>-48.5</v>
-      </c>
-      <c r="F21">
-        <v>-46.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-10</v>
       </c>
       <c r="B22">
+        <v>-49.8</v>
+      </c>
+      <c r="C22">
+        <v>-52.9</v>
+      </c>
+      <c r="D22">
         <v>-54</v>
       </c>
-      <c r="C22">
+      <c r="E22">
         <v>-57.3</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>-57.8</v>
       </c>
-      <c r="E22">
-        <v>-52.9</v>
-      </c>
-      <c r="F22">
-        <v>-49.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-12</v>
       </c>
       <c r="B23">
+        <v>-53.5</v>
+      </c>
+      <c r="C23">
+        <v>-57</v>
+      </c>
+      <c r="D23">
         <v>-60.8</v>
       </c>
-      <c r="C23">
+      <c r="E23">
         <v>-62.6</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>-63.9</v>
       </c>
-      <c r="E23">
-        <v>-57</v>
-      </c>
-      <c r="F23">
-        <v>-53.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-14</v>
       </c>
       <c r="B24">
+        <v>-60.4</v>
+      </c>
+      <c r="C24">
+        <v>-63.3</v>
+      </c>
+      <c r="D24">
         <v>-64.900000000000006</v>
       </c>
-      <c r="C24">
+      <c r="E24">
         <v>-68.3</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>-68.900000000000006</v>
       </c>
-      <c r="E24">
-        <v>-63.3</v>
-      </c>
-      <c r="F24">
-        <v>-60.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-16</v>
       </c>
       <c r="B25">
+        <v>-64.599999999999994</v>
+      </c>
+      <c r="C25">
+        <v>-70</v>
+      </c>
+      <c r="D25">
         <v>-72.400000000000006</v>
       </c>
-      <c r="C25">
+      <c r="E25">
         <v>-76.3</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>-74.5</v>
       </c>
-      <c r="E25">
-        <v>-70</v>
-      </c>
-      <c r="F25">
-        <v>-64.599999999999994</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-18</v>
       </c>
       <c r="B26">
+        <v>-70</v>
+      </c>
+      <c r="C26">
+        <v>-76.099999999999994</v>
+      </c>
+      <c r="D26">
         <v>-75.8</v>
       </c>
-      <c r="C26">
+      <c r="E26">
         <v>-82.4</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>-82.3</v>
       </c>
-      <c r="E26">
-        <v>-76.099999999999994</v>
-      </c>
-      <c r="F26">
-        <v>-70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-20</v>
       </c>
       <c r="B27">
+        <v>-75.900000000000006</v>
+      </c>
+      <c r="C27">
+        <v>-80.400000000000006</v>
+      </c>
+      <c r="D27">
         <v>-86.7</v>
       </c>
-      <c r="C27">
+      <c r="E27">
         <v>-90.2</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>-86.9</v>
       </c>
-      <c r="E27">
-        <v>-80.400000000000006</v>
-      </c>
-      <c r="F27">
-        <v>-75.900000000000006</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-22</v>
       </c>
       <c r="B28">
+        <v>-79.599999999999994</v>
+      </c>
+      <c r="C28">
+        <v>-86.5</v>
+      </c>
+      <c r="D28">
         <v>-92.6</v>
       </c>
-      <c r="C28">
+      <c r="E28">
         <v>-92.1</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>-95.5</v>
       </c>
-      <c r="E28">
-        <v>-86.5</v>
-      </c>
-      <c r="F28">
-        <v>-79.599999999999994</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-24</v>
       </c>
       <c r="B29">
+        <v>-86.1</v>
+      </c>
+      <c r="C29">
+        <v>-92.3</v>
+      </c>
+      <c r="D29">
         <v>-96.2</v>
       </c>
-      <c r="C29">
+      <c r="E29">
         <v>-100.4</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>-101.4</v>
       </c>
-      <c r="E29">
-        <v>-92.3</v>
-      </c>
-      <c r="F29">
-        <v>-86.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-26</v>
       </c>
       <c r="B30">
+        <v>-92.3</v>
+      </c>
+      <c r="C30">
+        <v>-98.4</v>
+      </c>
+      <c r="D30">
         <v>-102.4</v>
       </c>
-      <c r="C30">
+      <c r="E30">
         <v>-107.6</v>
       </c>
-      <c r="D30">
+      <c r="F30">
         <v>-106.9</v>
       </c>
-      <c r="E30">
-        <v>-98.4</v>
-      </c>
-      <c r="F30">
-        <v>-92.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-28</v>
       </c>
       <c r="B31">
+        <v>-99.1</v>
+      </c>
+      <c r="C31">
+        <v>-100.9</v>
+      </c>
+      <c r="D31">
         <v>-108.3</v>
       </c>
-      <c r="C31">
+      <c r="E31">
         <v>-114.9</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>-112.9</v>
       </c>
-      <c r="E31">
-        <v>-100.9</v>
-      </c>
-      <c r="F31">
-        <v>-99.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-30</v>
       </c>
       <c r="B32">
+        <v>-104.9</v>
+      </c>
+      <c r="C32">
+        <v>-107.2</v>
+      </c>
+      <c r="D32">
         <v>-115.6</v>
       </c>
-      <c r="C32">
+      <c r="E32">
         <v>-120.4</v>
       </c>
-      <c r="D32">
+      <c r="F32">
         <v>-122.2</v>
-      </c>
-      <c r="E32">
-        <v>-107.2</v>
-      </c>
-      <c r="F32">
-        <v>-104.9</v>
       </c>
     </row>
   </sheetData>
@@ -1126,33 +1126,33 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>-76.3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>28</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>-69</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>26</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>-66.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>-59.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>22</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>-54.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>-50.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>18</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>-45.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>-39.799999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>14</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>-31.8</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>-28.2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>-21.4</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>-11.3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>-6.8</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-2</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-4</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-6</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-8</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>28.2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-10</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-12</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-14</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>43.7</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-16</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>50.4</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-18</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>55.1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-20</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-22</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-24</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-26</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>77.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-28</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-30</v>
       </c>
@@ -1785,30 +1785,30 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1.6</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>65.2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-1.4</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>59.4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-1.2</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-0.8</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-0.6</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-0.4</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-0.2</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>-10.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.4</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>-19.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.6</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>-28.2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.8</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>-37</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>-45.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.2</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>-53.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.4</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -2114,26 +2114,26 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1.6</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>-56.9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-1.4</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>-51.6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-1.2</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>-44.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-0.999999999999999</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>-38.200000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-0.79999999999999905</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>-30.7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-0.6</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>-22.6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-0.4</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>-15.1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-0.2</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>-7.3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.4</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.6</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.8</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>33.9</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.2</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.4</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -2435,17 +2435,17 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.24</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>58.6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>117.2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.75</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>172.8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.24</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.5</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1.75</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2.2599999999999998</v>
       </c>
@@ -2534,27 +2534,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189972B0-DBD8-4ED5-AAD1-42754C13C545}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-30</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>-1.6060000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-28</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>-1.5109999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-26</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>-1.3560000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-24</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>-1.2729999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-22</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>-1.1970000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-20</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>-1.1279999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-18</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>-1.0149999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-16</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>-0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-14</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>-0.82599999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-12</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>-0.70399999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-10</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>-0.58399999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-8</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>-0.49299999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-6</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>-0.39700000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-4</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>-0.309</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-2</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>-0.21199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>-1.4E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>0.255</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>10</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>12</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>14</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>0.69399999999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>16</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>18</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>24</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>1.181</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>1.2569999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2904,37 +2904,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB01174-49A6-4102-B06C-928CAEE5085A}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E1">
         <v>0.25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>-6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0.16800000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0.42299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>18</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>21</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>24</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>27</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30</v>
       </c>
@@ -3066,21 +3066,21 @@
         <v>1.0840000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>-4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>0.224</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>12</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>15</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>0.76900000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>24</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>27</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>30</v>
       </c>
@@ -3212,21 +3212,21 @@
         <v>1.0860000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E27">
         <v>0.75</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>-4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>12</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>15</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>18</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>21</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>24</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>27</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -3358,21 +3358,21 @@
         <v>1.101</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>6</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0.23100000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>9</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>12</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>0.438</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>15</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>18</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>21</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>0.76900000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>24</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>27</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>1.018</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>30</v>
       </c>
@@ -3504,21 +3504,21 @@
         <v>1.1279999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E53">
         <v>1.25</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>6</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>0.186</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>9</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>0.30199999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>12</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>15</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>0.54900000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>18</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>21</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0.78700000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>24</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>27</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>0.99099999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>30</v>
       </c>
@@ -3650,21 +3650,21 @@
         <v>1.087</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E66">
         <v>1.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>0</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>-8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>3</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>6</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>9</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>0.31900000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>12</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>0.43099999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>15</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>0.56599999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>18</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>0.66200000000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>21</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>24</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>27</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>1.0069999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>30</v>
       </c>
@@ -3796,21 +3796,21 @@
         <v>1.093</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E79">
         <v>1.75</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>0</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>-8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>3</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>6</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>9</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>0.34899999999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>12</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>15</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>0.53700000000000003</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>18</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>21</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>0.75900000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>24</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>27</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>1.008</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>30</v>
       </c>
@@ -3942,21 +3942,21 @@
         <v>1.1339999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>0</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>-1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>3</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>6</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>0.224</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>9</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>0.312</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>12</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>15</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>0.56899999999999995</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>18</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>0.66400000000000003</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>21</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>24</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>27</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>30</v>
       </c>
@@ -4088,21 +4088,21 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B105" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D105" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E105">
         <v>2.25</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>0</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>-1.6E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>3</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>6</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>9</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>12</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>0.438</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>15</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>18</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>21</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>24</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>27</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>30</v>
       </c>
@@ -4234,21 +4234,21 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B118" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D118" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E118">
         <v>2.5</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>0</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>-1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>3</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>6</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>9</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>0.32700000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>12</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>15</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>0.57199999999999995</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>18</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>0.67800000000000005</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>21</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>0.78600000000000003</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>24</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>27</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>1.024</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>30</v>
       </c>
@@ -4380,24 +4380,24 @@
         <v>1.1339999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B132" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D132" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E132">
         <v>0.25</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>0</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>-8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>3</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>6</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>9</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>0.42699999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>12</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>15</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>18</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>0.876</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>21</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>24</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>1.1639999999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>27</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>1.3180000000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>30</v>
       </c>
@@ -4529,21 +4529,21 @@
         <v>1.486</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B145" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E145">
         <v>0.5</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>0</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>-8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>3</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>6</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>9</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>12</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>15</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>0.71799999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>18</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>21</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>1.0309999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>24</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>1.1819999999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>27</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>1.3240000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>30</v>
       </c>
@@ -4675,21 +4675,21 @@
         <v>1.4910000000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B158" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D158" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E158">
         <v>0.75</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>0</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>-7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>3</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>6</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>9</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>0.42799999999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>12</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>15</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>18</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>21</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>1.026</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>24</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>1.2050000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>27</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>30</v>
       </c>
@@ -4821,21 +4821,21 @@
         <v>1.518</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B171" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D171" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E171">
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>0</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>3</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>6</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>0.30199999999999999</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>9</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>0.42299999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>12</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>0.59299999999999997</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>15</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>18</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>21</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>1.0429999999999999</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>24</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>1.1679999999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>27</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>1.343</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>30</v>
       </c>
@@ -4967,21 +4967,21 @@
         <v>1.506</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B184" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D184" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E184">
         <v>1.25</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>0</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>3</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>6</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>9</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>12</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>15</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>18</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>21</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>24</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>1.165</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>27</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>1.2889999999999999</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>30</v>
       </c>
@@ -5113,21 +5113,21 @@
         <v>1.5169999999999999</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B197" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D197" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E197">
         <v>1.5</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>0</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>3</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>6</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>9</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>12</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>15</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>18</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>21</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>1.0509999999999999</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>24</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>1.1970000000000001</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>27</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>1.3640000000000001</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>30</v>
       </c>
@@ -5259,21 +5259,21 @@
         <v>1.5229999999999999</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B210" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D210" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E210">
         <v>1.75</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>0</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>3</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>6</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>9</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>0.42199999999999999</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>12</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>0.59299999999999997</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>15</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>18</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>21</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>24</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>1.2470000000000001</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>27</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>1.361</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>30</v>
       </c>
@@ -5405,21 +5405,21 @@
         <v>1.536</v>
       </c>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B223" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D223" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E223">
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>0</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>-0.02</v>
       </c>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>3</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>6</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>0.251</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>9</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>12</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>15</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>0.76200000000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>18</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>21</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>1.0349999999999999</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>24</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>1.2110000000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>27</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>1.381</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>30</v>
       </c>
@@ -5551,21 +5551,21 @@
         <v>1.546</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B236" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D236" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E236">
         <v>2.25</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>0</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>-1.9E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>3</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>6</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>0.26900000000000002</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>9</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>0.437</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>12</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>15</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>18</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>21</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>1.0680000000000001</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>24</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>1.244</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>27</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>30</v>
       </c>
@@ -5697,21 +5697,21 @@
         <v>1.5860000000000001</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B249" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D249" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E249">
         <v>2.5</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>0</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>-4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>3</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>6</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>9</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>0.439</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>12</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="255" spans="1:5">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>15</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>18</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>0.95799999999999996</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>21</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>1.0609999999999999</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>24</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>1.2330000000000001</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>27</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>1.3779999999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Act 3.1 con datos de Nicolas
</commit_message>
<xml_diff>
--- a/Efecto Hall/Efecto_Hall.xlsx
+++ b/Efecto Hall/Efecto_Hall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiaalvarezlopez/Documents/Universidad/Noveno Semestre/Laboratorio Intermedio/Laboratorios/Efecto Hall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9872A3BC-3590-D546-BFEA-FD1E913F5CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728B396C-C099-1D42-B8D1-F06DFB06E239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="980" windowWidth="28500" windowHeight="16180" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p V-I" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,10 @@
     <sheet name="n V-B" sheetId="8" r:id="rId4"/>
     <sheet name="B-I" sheetId="3" r:id="rId5"/>
     <sheet name="Voltaje longitudinal" sheetId="6" r:id="rId6"/>
-    <sheet name="Voltaje long 2" sheetId="7" r:id="rId7"/>
+    <sheet name="Datos Nicolas" sheetId="11" r:id="rId7"/>
+    <sheet name="Voltaje long 2" sheetId="7" r:id="rId8"/>
+    <sheet name="Voltaje longitudinal p" sheetId="10" r:id="rId9"/>
+    <sheet name="Voltaje longitudinal n" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
   <si>
     <t>Corriente (mA)</t>
   </si>
@@ -98,11 +101,47 @@
   <si>
     <t>Voltaje Hall a 2 A (mV)</t>
   </si>
+  <si>
+    <t>B = 25 (mT)</t>
+  </si>
+  <si>
+    <t>B = 50 (mT)</t>
+  </si>
+  <si>
+    <t>B = 75 (mT)</t>
+  </si>
+  <si>
+    <t>B = 100 (mT)</t>
+  </si>
+  <si>
+    <t>B = 125 (mT)</t>
+  </si>
+  <si>
+    <t>B = 150 (mT)</t>
+  </si>
+  <si>
+    <t>B = 175 (mT)</t>
+  </si>
+  <si>
+    <t>B = 225 (mT)</t>
+  </si>
+  <si>
+    <t>B = 250 (mT)</t>
+  </si>
+  <si>
+    <t>B = 275 (mT)</t>
+  </si>
+  <si>
+    <t>Corriente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +164,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -134,13 +185,193 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1115,6 +1346,804 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E7381E-BF4A-534D-AA3A-AD86D5EB2108}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>-30</v>
+      </c>
+      <c r="B2" s="6">
+        <v>-1.1191944339239059</v>
+      </c>
+      <c r="C2" s="7">
+        <v>-1.1202302059708877</v>
+      </c>
+      <c r="D2" s="7">
+        <v>-1.1208458691754897</v>
+      </c>
+      <c r="E2" s="7">
+        <v>-1.1230065380965129</v>
+      </c>
+      <c r="F2" s="7">
+        <v>-1.1247632952631492</v>
+      </c>
+      <c r="G2" s="7">
+        <v>-1.1264083124224922</v>
+      </c>
+      <c r="H2" s="7">
+        <v>-1.1280752285199369</v>
+      </c>
+      <c r="I2" s="7">
+        <v>-1.1298188785510308</v>
+      </c>
+      <c r="J2" s="7">
+        <v>-1.1330889994369679</v>
+      </c>
+      <c r="K2" s="8">
+        <v>-1.1381130227571363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>-27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>-1.0078131151650569</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-1.0079174981548014</v>
+      </c>
+      <c r="D3" s="10">
+        <v>-1.0089090105373055</v>
+      </c>
+      <c r="E3" s="10">
+        <v>-1.0108752299653434</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-1.0120769935348246</v>
+      </c>
+      <c r="G3" s="10">
+        <v>-1.0135023047388658</v>
+      </c>
+      <c r="H3" s="10">
+        <v>-1.0154115639634347</v>
+      </c>
+      <c r="I3" s="10">
+        <v>-1.0173648818309564</v>
+      </c>
+      <c r="J3" s="10">
+        <v>-1.0200814968947021</v>
+      </c>
+      <c r="K3" s="11">
+        <v>-1.0241764813919634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>-24</v>
+      </c>
+      <c r="B4" s="9">
+        <v>-0.89603817594372637</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-0.89605662080278725</v>
+      </c>
+      <c r="D4" s="10">
+        <v>-0.8969230193997153</v>
+      </c>
+      <c r="E4" s="10">
+        <v>-0.89850351399428108</v>
+      </c>
+      <c r="F4" s="10">
+        <v>-0.89946196200829187</v>
+      </c>
+      <c r="G4" s="10">
+        <v>-0.90062657703504378</v>
+      </c>
+      <c r="H4" s="10">
+        <v>-0.90224209202359162</v>
+      </c>
+      <c r="I4" s="10">
+        <v>-0.90404493928372165</v>
+      </c>
+      <c r="J4" s="10">
+        <v>-0.90659249958061794</v>
+      </c>
+      <c r="K4" s="11">
+        <v>-0.91020489699926677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>-21</v>
+      </c>
+      <c r="B5" s="9">
+        <v>-0.78369606246842238</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-0.78425348888986346</v>
+      </c>
+      <c r="D5" s="10">
+        <v>-0.78492571781271347</v>
+      </c>
+      <c r="E5" s="10">
+        <v>-0.78588116843559253</v>
+      </c>
+      <c r="F5" s="10">
+        <v>-0.78708342836285849</v>
+      </c>
+      <c r="G5" s="10">
+        <v>-0.7879479559941962</v>
+      </c>
+      <c r="H5" s="10">
+        <v>-0.78999277118030919</v>
+      </c>
+      <c r="I5" s="10">
+        <v>-0.79131930003489948</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-0.79346361195398163</v>
+      </c>
+      <c r="K5" s="11">
+        <v>-0.79657236891012417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>-18</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-0.67201923619622472</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-0.67215746215999728</v>
+      </c>
+      <c r="D6" s="10">
+        <v>-0.67275413643392235</v>
+      </c>
+      <c r="E6" s="10">
+        <v>-0.67378692261613204</v>
+      </c>
+      <c r="F6" s="10">
+        <v>-0.67492483996580388</v>
+      </c>
+      <c r="G6" s="10">
+        <v>-0.67568025508609852</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-0.67690577007139141</v>
+      </c>
+      <c r="I6" s="10">
+        <v>-0.67789036725242213</v>
+      </c>
+      <c r="J6" s="10">
+        <v>-0.67999650251681021</v>
+      </c>
+      <c r="K6" s="11">
+        <v>-0.68276948436074991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>-15</v>
+      </c>
+      <c r="B7" s="9">
+        <v>-0.55979053865870776</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-0.56021867456295682</v>
+      </c>
+      <c r="D7" s="10">
+        <v>-0.56045157295456283</v>
+      </c>
+      <c r="E7" s="10">
+        <v>-0.56156834387689458</v>
+      </c>
+      <c r="F7" s="10">
+        <v>-0.56236371807473007</v>
+      </c>
+      <c r="G7" s="10">
+        <v>-0.56311170582493175</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-0.56415010625217132</v>
+      </c>
+      <c r="I7" s="10">
+        <v>-0.56491680314317383</v>
+      </c>
+      <c r="J7" s="10">
+        <v>-0.56688317117969766</v>
+      </c>
+      <c r="K7" s="11">
+        <v>-0.56892125402683835</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>-12</v>
+      </c>
+      <c r="B8" s="9">
+        <v>-0.44796158260645025</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-0.44800305846177374</v>
+      </c>
+      <c r="D8" s="10">
+        <v>-0.44834421505398259</v>
+      </c>
+      <c r="E8" s="10">
+        <v>-0.44929075496775867</v>
+      </c>
+      <c r="F8" s="10">
+        <v>-0.44969443566460132</v>
+      </c>
+      <c r="G8" s="10">
+        <v>-0.45045160651170474</v>
+      </c>
+      <c r="H8" s="10">
+        <v>-0.4513199274925685</v>
+      </c>
+      <c r="I8" s="10">
+        <v>-0.4521451645336384</v>
+      </c>
+      <c r="J8" s="10">
+        <v>-0.45326049366408228</v>
+      </c>
+      <c r="K8" s="11">
+        <v>-0.45511085314358241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>-9</v>
+      </c>
+      <c r="B9" s="9">
+        <v>-0.33598006929440383</v>
+      </c>
+      <c r="C9" s="10">
+        <v>-0.33611387721958558</v>
+      </c>
+      <c r="D9" s="10">
+        <v>-0.33629809408309969</v>
+      </c>
+      <c r="E9" s="10">
+        <v>-0.33697357383913362</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-0.33731393050514974</v>
+      </c>
+      <c r="G9" s="10">
+        <v>-0.33800445233280108</v>
+      </c>
+      <c r="H9" s="10">
+        <v>-0.33843595753108013</v>
+      </c>
+      <c r="I9" s="10">
+        <v>-0.33893346322310303</v>
+      </c>
+      <c r="J9" s="10">
+        <v>-0.34006178172568169</v>
+      </c>
+      <c r="K9" s="11">
+        <v>-0.34134914027710628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>-6</v>
+      </c>
+      <c r="B10" s="9">
+        <v>-0.22387421509787761</v>
+      </c>
+      <c r="C10" s="10">
+        <v>-0.22396779870453429</v>
+      </c>
+      <c r="D10" s="10">
+        <v>-0.22427467905439888</v>
+      </c>
+      <c r="E10" s="10">
+        <v>-0.2245937968143307</v>
+      </c>
+      <c r="F10" s="10">
+        <v>-0.22501122314528943</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-0.22532712067641283</v>
+      </c>
+      <c r="H10" s="10">
+        <v>-0.22560383848177196</v>
+      </c>
+      <c r="I10" s="10">
+        <v>-0.22602863992181518</v>
+      </c>
+      <c r="J10" s="10">
+        <v>-0.22671193752330612</v>
+      </c>
+      <c r="K10" s="11">
+        <v>-0.22765766219973113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>-3</v>
+      </c>
+      <c r="B11" s="9">
+        <v>-0.11196394920980758</v>
+      </c>
+      <c r="C11" s="10">
+        <v>-0.11201489214332717</v>
+      </c>
+      <c r="D11" s="10">
+        <v>-0.11211388103956665</v>
+      </c>
+      <c r="E11" s="10">
+        <v>-0.11233295025453641</v>
+      </c>
+      <c r="F11" s="10">
+        <v>-0.11242640231796397</v>
+      </c>
+      <c r="G11" s="10">
+        <v>-0.11262065836646359</v>
+      </c>
+      <c r="H11" s="10">
+        <v>-0.1128238706256601</v>
+      </c>
+      <c r="I11" s="10">
+        <v>-0.11301678389945134</v>
+      </c>
+      <c r="J11" s="10">
+        <v>-0.11335603065004378</v>
+      </c>
+      <c r="K11" s="11">
+        <v>-0.11381391538570713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.11194402214097453</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.11200797824954348</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.11212317262707613</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.1123013418995179</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.11243754397178847</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.11258239907294458</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.11280216667545082</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.11303499595580845</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.11334458478439557</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.11385241581458756</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.22391485037410888</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.22397533072449355</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.22427210461668029</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.22459012018819038</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.22501681836681972</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.22526731162532179</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.22568529985671493</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.22601179671012228</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.22678827681299346</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.22760448902716507</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>9</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.33578941514203109</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.33608103665889927</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.33641161207015102</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.33682425849488351</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.33725587339627711</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.33787634378950698</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.33848032420084251</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.33902407301957477</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.34011188462251468</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.34139173479617657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.44787440799285189</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.44799296545397066</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.44854534286674286</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.44933874676658586</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.44995115660846702</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.45045518006562363</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.45134887108050487</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.45212948848214224</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.45354821997965022</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.45511554811808946</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.55975561060438095</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.56007113364683014</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.56050666729776133</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.56168863643096734</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.56224445880927532</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.56328915323133288</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.56388045133357523</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.56504513568410253</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0.56673634189544408</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.56912749427449194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>18</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.67163488687562123</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.6723604990506673</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.67272818903863807</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.67398848540957945</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.67484468302906453</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.67567781796545834</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.67697032123651202</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.67782726480868183</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0.67986760973156446</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.68282285851271363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>21</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.78406468707199273</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.7839569221328706</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.78479944467937512</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.78632791255395995</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0.7871683023975663</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.78815900284194451</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.79010707741058328</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.79121603230589188</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0.79351212804042337</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.79635990521723021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>24</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.89528774537212352</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.89582551096601415</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.89688506697690662</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.89813330974232464</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.89978826591234773</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.9009968601688888</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.90238893300773826</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0.90425616262776132</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0.90692139308834974</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0.91030507456808796</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>27</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1.0076010924364587</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1.0079654181623947</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1.0087376107681612</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1.0109151105307612</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1.0119722375414628</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1.0133855928284212</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1.0155913299252906</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1.0168605370407371</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1.0206328898663184</v>
+      </c>
+      <c r="K21" s="11">
+        <v>1.0243193557977539</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>30</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1.119895346866584</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1.1203661891434602</v>
+      </c>
+      <c r="D22" s="14">
+        <v>1.1208612034903176</v>
+      </c>
+      <c r="E22" s="14">
+        <v>1.122662091819826</v>
+      </c>
+      <c r="F22" s="14">
+        <v>1.1247167887295437</v>
+      </c>
+      <c r="G22" s="14">
+        <v>1.126251812066086</v>
+      </c>
+      <c r="H22" s="14">
+        <v>1.1281106629239854</v>
+      </c>
+      <c r="I22" s="14">
+        <v>1.1304544498904858</v>
+      </c>
+      <c r="J22" s="14">
+        <v>1.1334081756803762</v>
+      </c>
+      <c r="K22" s="15">
+        <v>1.1379584663079358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE97E303-9B46-48BF-B4E7-CA9F74346ADA}">
   <dimension ref="A1:F32"/>
@@ -2110,7 +3139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B7489-1182-4D28-9ACB-C8169A464B73}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E18"/>
     </sheetView>
   </sheetViews>
@@ -2540,12 +3569,14 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2906,17 +3937,277 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC191A8D-AE50-FC41-94B4-A2F288638FA7}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>-30</v>
+      </c>
+      <c r="B2" s="19">
+        <v>-1.1190330287635815</v>
+      </c>
+      <c r="C2" s="19">
+        <v>-1.0648490394346599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>-27</v>
+      </c>
+      <c r="B3" s="20">
+        <v>-1.007392863505443</v>
+      </c>
+      <c r="C3" s="20">
+        <v>-0.95844732573193892</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>-24</v>
+      </c>
+      <c r="B4" s="20">
+        <v>-0.89514226934954333</v>
+      </c>
+      <c r="C4" s="20">
+        <v>-0.85239190776329965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>-21</v>
+      </c>
+      <c r="B5" s="20">
+        <v>-0.78339161992153417</v>
+      </c>
+      <c r="C5" s="20">
+        <v>-0.74544997340422625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>-18</v>
+      </c>
+      <c r="B6" s="20">
+        <v>-0.67150379175444297</v>
+      </c>
+      <c r="C6" s="20">
+        <v>-0.63894128526170002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>-15</v>
+      </c>
+      <c r="B7" s="20">
+        <v>-0.55946802073108559</v>
+      </c>
+      <c r="C7" s="20">
+        <v>-0.53247337431877739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>-12</v>
+      </c>
+      <c r="B8" s="20">
+        <v>-0.44751035231432057</v>
+      </c>
+      <c r="C8" s="20">
+        <v>-0.4260367667978221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>-9</v>
+      </c>
+      <c r="B9" s="20">
+        <v>-0.33565087471767341</v>
+      </c>
+      <c r="C9" s="20">
+        <v>-0.31964815567146654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>-6</v>
+      </c>
+      <c r="B10" s="20">
+        <v>-0.22377180963066384</v>
+      </c>
+      <c r="C10" s="20">
+        <v>-0.21296616015400313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>-3</v>
+      </c>
+      <c r="B11" s="20">
+        <v>-0.11193593135575312</v>
+      </c>
+      <c r="C11" s="20">
+        <v>-0.10650268047248286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>0</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0.11190779269828896</v>
+      </c>
+      <c r="C13" s="20">
+        <v>0.10655067298668507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14" s="20">
+        <v>0.22378156923132964</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0.21298207823984286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>9</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0.33568643984295293</v>
+      </c>
+      <c r="C15" s="20">
+        <v>0.31953611107992841</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="20">
+        <v>0.4473970915474848</v>
+      </c>
+      <c r="C16" s="20">
+        <v>0.42604055568304422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="20">
+        <v>0.55932929661087494</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0.53262842505217023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>18</v>
+      </c>
+      <c r="B18" s="20">
+        <v>0.67109484432695832</v>
+      </c>
+      <c r="C18" s="20">
+        <v>0.63908464347487592</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>21</v>
+      </c>
+      <c r="B19" s="20">
+        <v>0.78338868828714803</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0.74542846320294509</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>24</v>
+      </c>
+      <c r="B20" s="20">
+        <v>0.89551256753868225</v>
+      </c>
+      <c r="C20" s="20">
+        <v>0.8521848129890508</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>27</v>
+      </c>
+      <c r="B21" s="20">
+        <v>1.0073296488843138</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.95862061840614254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>30</v>
+      </c>
+      <c r="B22" s="21">
+        <v>1.1191924140873153</v>
+      </c>
+      <c r="C22" s="21">
+        <v>1.0653242338593716</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB01174-49A6-4102-B06C-928CAEE5085A}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C250" sqref="C250:C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -5851,4 +7142,801 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E72A9C4-D5E7-2E4F-9489-816A9C988AF6}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="A23:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>-30</v>
+      </c>
+      <c r="B2" s="6">
+        <v>-1.0653093663891799</v>
+      </c>
+      <c r="C2" s="7">
+        <v>-1.0660378219279871</v>
+      </c>
+      <c r="D2" s="7">
+        <v>-1.0672342644621551</v>
+      </c>
+      <c r="E2" s="7">
+        <v>-1.0689070039614008</v>
+      </c>
+      <c r="F2" s="7">
+        <v>-1.0701250675173064</v>
+      </c>
+      <c r="G2" s="7">
+        <v>-1.0720665519140087</v>
+      </c>
+      <c r="H2" s="7">
+        <v>-1.0739137105102425</v>
+      </c>
+      <c r="I2" s="7">
+        <v>-1.0752709786188093</v>
+      </c>
+      <c r="J2" s="7">
+        <v>-1.0788081165430661</v>
+      </c>
+      <c r="K2" s="8">
+        <v>-1.0828762922977726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>-27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>-0.95907983981933143</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-0.95909435956522493</v>
+      </c>
+      <c r="D3" s="10">
+        <v>-0.96026435507765007</v>
+      </c>
+      <c r="E3" s="10">
+        <v>-0.96230182805997999</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-0.96299999858959207</v>
+      </c>
+      <c r="G3" s="10">
+        <v>-0.964892560209759</v>
+      </c>
+      <c r="H3" s="10">
+        <v>-0.96657154119504174</v>
+      </c>
+      <c r="I3" s="10">
+        <v>-0.96787066338981376</v>
+      </c>
+      <c r="J3" s="10">
+        <v>-0.97088568916659646</v>
+      </c>
+      <c r="K3" s="11">
+        <v>-0.97451512305572074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>-24</v>
+      </c>
+      <c r="B4" s="9">
+        <v>-0.85231009609478259</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-0.85256994793816276</v>
+      </c>
+      <c r="D4" s="10">
+        <v>-0.8534650098742157</v>
+      </c>
+      <c r="E4" s="10">
+        <v>-0.85511699033150135</v>
+      </c>
+      <c r="F4" s="10">
+        <v>-0.85635000372308479</v>
+      </c>
+      <c r="G4" s="10">
+        <v>-0.85768840513460032</v>
+      </c>
+      <c r="H4" s="10">
+        <v>-0.85900717394671366</v>
+      </c>
+      <c r="I4" s="10">
+        <v>-0.86059431056945346</v>
+      </c>
+      <c r="J4" s="10">
+        <v>-0.86311651985002436</v>
+      </c>
+      <c r="K4" s="11">
+        <v>-0.86652106573563681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>-21</v>
+      </c>
+      <c r="B5" s="9">
+        <v>-0.74587202333762204</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-0.74597942995994015</v>
+      </c>
+      <c r="D5" s="10">
+        <v>-0.74708234267708062</v>
+      </c>
+      <c r="E5" s="10">
+        <v>-0.74836816535979778</v>
+      </c>
+      <c r="F5" s="10">
+        <v>-0.7493997138372398</v>
+      </c>
+      <c r="G5" s="10">
+        <v>-0.75025564517005361</v>
+      </c>
+      <c r="H5" s="10">
+        <v>-0.75168441497283223</v>
+      </c>
+      <c r="I5" s="10">
+        <v>-0.75278059568054123</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-0.75537000912047569</v>
+      </c>
+      <c r="K5" s="11">
+        <v>-0.75828814728769489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>-18</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-0.6393230186469151</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-0.6397397971566734</v>
+      </c>
+      <c r="D6" s="10">
+        <v>-0.64011402598806211</v>
+      </c>
+      <c r="E6" s="10">
+        <v>-0.64133739465541095</v>
+      </c>
+      <c r="F6" s="10">
+        <v>-0.64222812039787125</v>
+      </c>
+      <c r="G6" s="10">
+        <v>-0.64321033821217555</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-0.64444215675227579</v>
+      </c>
+      <c r="I6" s="10">
+        <v>-0.645322829053803</v>
+      </c>
+      <c r="J6" s="10">
+        <v>-0.6471330913536365</v>
+      </c>
+      <c r="K6" s="11">
+        <v>-0.64982739686030822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>-15</v>
+      </c>
+      <c r="B7" s="9">
+        <v>-0.53288676356254061</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-0.533176262735092</v>
+      </c>
+      <c r="D7" s="10">
+        <v>-0.53362233549077098</v>
+      </c>
+      <c r="E7" s="10">
+        <v>-0.53458453983137666</v>
+      </c>
+      <c r="F7" s="10">
+        <v>-0.5353145508066286</v>
+      </c>
+      <c r="G7" s="10">
+        <v>-0.53602773266804038</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-0.53691201192206472</v>
+      </c>
+      <c r="I7" s="10">
+        <v>-0.5378680232888452</v>
+      </c>
+      <c r="J7" s="10">
+        <v>-0.53951925507617859</v>
+      </c>
+      <c r="K7" s="11">
+        <v>-0.54141129443011626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>-12</v>
+      </c>
+      <c r="B8" s="9">
+        <v>-0.42612142608657749</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-0.42647247260192495</v>
+      </c>
+      <c r="D8" s="10">
+        <v>-0.42677672471508865</v>
+      </c>
+      <c r="E8" s="10">
+        <v>-0.42761171127956843</v>
+      </c>
+      <c r="F8" s="10">
+        <v>-0.42812818416548076</v>
+      </c>
+      <c r="G8" s="10">
+        <v>-0.42862327760594515</v>
+      </c>
+      <c r="H8" s="10">
+        <v>-0.42947000633157356</v>
+      </c>
+      <c r="I8" s="10">
+        <v>-0.43020999142582894</v>
+      </c>
+      <c r="J8" s="10">
+        <v>-0.43161818996613099</v>
+      </c>
+      <c r="K8" s="11">
+        <v>-0.43323650316280049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>-9</v>
+      </c>
+      <c r="B9" s="9">
+        <v>-0.31960706531004268</v>
+      </c>
+      <c r="C9" s="10">
+        <v>-0.31979204041749343</v>
+      </c>
+      <c r="D9" s="10">
+        <v>-0.32012929541263035</v>
+      </c>
+      <c r="E9" s="10">
+        <v>-0.32079397786299219</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-0.32104723285057785</v>
+      </c>
+      <c r="G9" s="10">
+        <v>-0.32161182736292954</v>
+      </c>
+      <c r="H9" s="10">
+        <v>-0.32204759423937657</v>
+      </c>
+      <c r="I9" s="10">
+        <v>-0.32256453846737787</v>
+      </c>
+      <c r="J9" s="10">
+        <v>-0.32370603463631514</v>
+      </c>
+      <c r="K9" s="11">
+        <v>-0.32491183545180191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>-6</v>
+      </c>
+      <c r="B10" s="9">
+        <v>-0.21310169062229814</v>
+      </c>
+      <c r="C10" s="10">
+        <v>-0.21325784683242013</v>
+      </c>
+      <c r="D10" s="10">
+        <v>-0.21343169012192528</v>
+      </c>
+      <c r="E10" s="10">
+        <v>-0.21376084442008472</v>
+      </c>
+      <c r="F10" s="10">
+        <v>-0.2140479278939334</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-0.21434570434915287</v>
+      </c>
+      <c r="H10" s="10">
+        <v>-0.21480972639951146</v>
+      </c>
+      <c r="I10" s="10">
+        <v>-0.2151187950448763</v>
+      </c>
+      <c r="J10" s="10">
+        <v>-0.21569884952937474</v>
+      </c>
+      <c r="K10" s="11">
+        <v>-0.21659856792504964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>-3</v>
+      </c>
+      <c r="B11" s="9">
+        <v>-0.10655272361288447</v>
+      </c>
+      <c r="C11" s="10">
+        <v>-0.10662229205446368</v>
+      </c>
+      <c r="D11" s="10">
+        <v>-0.10668830614819322</v>
+      </c>
+      <c r="E11" s="10">
+        <v>-0.10689160128666825</v>
+      </c>
+      <c r="F11" s="10">
+        <v>-0.10705393319979295</v>
+      </c>
+      <c r="G11" s="10">
+        <v>-0.10720413580561054</v>
+      </c>
+      <c r="H11" s="10">
+        <v>-0.10738965246459514</v>
+      </c>
+      <c r="I11" s="10">
+        <v>-0.1075690507611355</v>
+      </c>
+      <c r="J11" s="10">
+        <v>-0.10787966733712887</v>
+      </c>
+      <c r="K11" s="11">
+        <v>-0.10830809072431995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.10657746581749449</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.10665547065328417</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.10672615609691552</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.10686955589675191</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.10703222857469837</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.10716140901025559</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.107394255334779</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.10756372137069796</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.10786815126776803</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.10827202211912887</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.21309348961383331</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.21327871990007322</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.21350927142741485</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.21383481390184123</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.21402652169788638</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.21432574899879717</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.21474899902091144</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.21508874035238715</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.21583787944360769</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.21653438549808396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>9</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.31968718177609379</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.31980253074368825</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.32012311015501083</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.32056378331247332</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.32108112246522985</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.32150605416637823</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.32220736868106958</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.32276374040925182</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.32378146213944686</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.32484387050529373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.42625229666683045</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.42624043716194676</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.42691413969517356</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.42752388663949231</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.42802226072049793</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.42877181656813779</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.42946129121617099</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.4302641443177187</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.43151969396021961</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.43332790829642864</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.53293501084324779</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.53303523929275265</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.5335895394384228</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.5344101286115196</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.53506179385426089</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.53593402910498711</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.53681921312276992</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.5379810434298351</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0.53952335492054782</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.54142306915999883</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>18</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.63942086422379152</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.63972081668470882</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.64035443811304626</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.6416085500740597</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.64197052319375025</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.64304024712474539</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.64401901775039672</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.6453360543192691</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0.64753626297349454</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.65012941415297087</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>21</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.74581230485225447</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.74647426439122733</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.7469640798163466</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.74804645891537125</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0.74922245842257917</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.75028711079606392</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.75189196997430541</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.75261868994038073</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0.75538756265274987</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.7580490402658443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>24</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.85207474424926</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.85303808406525761</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.85404228539889171</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.85514674531787827</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.85616246505771154</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.85734584886542287</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.85918392185242631</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0.86038071791837267</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0.86304391059648267</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0.86635674568412013</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>27</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.95914515036193937</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.95946700091608206</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.96046427381020594</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.96196486505299483</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0.96331764601560566</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0.96465904833668792</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.96632345144129095</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0.96796197624474134</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0.97096854273163635</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0.97479305768461855</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>30</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1.0655428665386457</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1.0659957769228026</v>
+      </c>
+      <c r="D22" s="14">
+        <v>1.0672947773804273</v>
+      </c>
+      <c r="E22" s="14">
+        <v>1.0689716114969299</v>
+      </c>
+      <c r="F22" s="14">
+        <v>1.0699083960660962</v>
+      </c>
+      <c r="G22" s="14">
+        <v>1.0718981265934695</v>
+      </c>
+      <c r="H22" s="14">
+        <v>1.0735033953383251</v>
+      </c>
+      <c r="I22" s="14">
+        <v>1.0757659461143945</v>
+      </c>
+      <c r="J22" s="14">
+        <v>1.0791583210897464</v>
+      </c>
+      <c r="K22" s="15">
+        <v>1.08302688119459</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>